<commit_message>
tooltip to ms C added
</commit_message>
<xml_diff>
--- a/codices.xlsx
+++ b/codices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olga/R_Workflow/philebus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE00204-0C1F-6E48-98E2-7952A67D0FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F8CD15-0A45-AB44-8D98-0C8EC6F4BA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
   <si>
     <t>url</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>Добавление к "Кратилу" есть в W (437e), но отсутствует в Q.</t>
+  </si>
+  <si>
+    <t>Не зависит от B.</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -1390,6 +1393,9 @@
       <c r="G7" t="s">
         <v>41</v>
       </c>
+      <c r="H7" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">

</xml_diff>